<commit_message>
change write.csv to write_csv to fix ncol error in completed template files
</commit_message>
<xml_diff>
--- a/raw_excel_pretest/test_pretest_1.xlsx
+++ b/raw_excel_pretest/test_pretest_1.xlsx
@@ -8,17 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hava\Documents\R\plater-prep\raw_excel_pretest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DCE7CB9-014C-4F6E-9C8A-107CFA4FAF28}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73E6DDD4-CA4A-4D84-8D1A-F10DA417BE3D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15" yWindow="-16020" windowWidth="18450" windowHeight="10575" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10290" yWindow="-5895" windowWidth="17280" windowHeight="8970" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="3-rr120-7-bc" sheetId="1" r:id="rId1"/>
     <sheet name="4-rr120-7-np" sheetId="2" r:id="rId2"/>
     <sheet name="7-sw61-7-bc" sheetId="3" r:id="rId3"/>
     <sheet name="8-sw61-7-np" sheetId="4" r:id="rId4"/>
-    <sheet name="6-sw61-6.5-np" sheetId="5" r:id="rId5"/>
-    <sheet name="5-sw61-6.5-bc" sheetId="6" r:id="rId6"/>
+    <sheet name="5-sw61-6.5-bc" sheetId="6" r:id="rId5"/>
+    <sheet name="6-sw61-6.5-np" sheetId="5" r:id="rId6"/>
     <sheet name="1-rr120-8-bc" sheetId="7" r:id="rId7"/>
     <sheet name="2-rr120-8-np" sheetId="8" r:id="rId8"/>
   </sheets>
@@ -2387,7 +2387,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A2:O34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
@@ -2934,6 +2934,556 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A2:O34"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.6640625" style="21" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" style="21" customWidth="1"/>
+    <col min="3" max="16384" width="9.109375" style="21"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="21" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="21" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="21" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="21" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="21" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="21" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="22">
+        <v>44019</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="21" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="23">
+        <v>0.55675925925925929</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="21" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="21" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="21" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="25"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="21" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="21" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" s="21" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B16" s="21" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B17" s="21" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B18" s="21" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B19" s="21" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B20" s="21" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B21" s="21" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A23" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="B23" s="25"/>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A24" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="B24" s="21">
+        <v>23.5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="B26" s="26"/>
+      <c r="C26" s="27">
+        <v>1</v>
+      </c>
+      <c r="D26" s="27">
+        <v>2</v>
+      </c>
+      <c r="E26" s="27">
+        <v>3</v>
+      </c>
+      <c r="F26" s="27">
+        <v>4</v>
+      </c>
+      <c r="G26" s="27">
+        <v>5</v>
+      </c>
+      <c r="H26" s="27">
+        <v>6</v>
+      </c>
+      <c r="I26" s="27">
+        <v>7</v>
+      </c>
+      <c r="J26" s="27">
+        <v>8</v>
+      </c>
+      <c r="K26" s="27">
+        <v>9</v>
+      </c>
+      <c r="L26" s="27">
+        <v>10</v>
+      </c>
+      <c r="M26" s="27">
+        <v>11</v>
+      </c>
+      <c r="N26" s="27">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" ht="19.2" x14ac:dyDescent="0.25">
+      <c r="B27" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="C27" s="28">
+        <v>720</v>
+      </c>
+      <c r="D27" s="28">
+        <v>786</v>
+      </c>
+      <c r="E27" s="28">
+        <v>442</v>
+      </c>
+      <c r="F27" s="28">
+        <v>458</v>
+      </c>
+      <c r="G27" s="30">
+        <v>1970</v>
+      </c>
+      <c r="H27" s="40">
+        <v>2525</v>
+      </c>
+      <c r="I27" s="28">
+        <v>457</v>
+      </c>
+      <c r="J27" s="28">
+        <v>562</v>
+      </c>
+      <c r="K27" s="40">
+        <v>2892</v>
+      </c>
+      <c r="L27" s="33">
+        <v>15462</v>
+      </c>
+      <c r="M27" s="28">
+        <v>125</v>
+      </c>
+      <c r="N27" s="28">
+        <v>61</v>
+      </c>
+      <c r="O27" s="35" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" ht="19.2" x14ac:dyDescent="0.25">
+      <c r="B28" s="27" t="s">
+        <v>31</v>
+      </c>
+      <c r="C28" s="28">
+        <v>586</v>
+      </c>
+      <c r="D28" s="28">
+        <v>565</v>
+      </c>
+      <c r="E28" s="28">
+        <v>385</v>
+      </c>
+      <c r="F28" s="28">
+        <v>375</v>
+      </c>
+      <c r="G28" s="40">
+        <v>3218</v>
+      </c>
+      <c r="H28" s="39">
+        <v>4203</v>
+      </c>
+      <c r="I28" s="28">
+        <v>528</v>
+      </c>
+      <c r="J28" s="28">
+        <v>477</v>
+      </c>
+      <c r="K28" s="40">
+        <v>2484</v>
+      </c>
+      <c r="L28" s="33">
+        <v>14460</v>
+      </c>
+      <c r="M28" s="28">
+        <v>127</v>
+      </c>
+      <c r="N28" s="28">
+        <v>63</v>
+      </c>
+      <c r="O28" s="35" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" ht="19.2" x14ac:dyDescent="0.25">
+      <c r="B29" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="C29" s="28">
+        <v>419</v>
+      </c>
+      <c r="D29" s="28">
+        <v>444</v>
+      </c>
+      <c r="E29" s="28">
+        <v>301</v>
+      </c>
+      <c r="F29" s="28">
+        <v>304</v>
+      </c>
+      <c r="G29" s="30">
+        <v>2210</v>
+      </c>
+      <c r="H29" s="40">
+        <v>2780</v>
+      </c>
+      <c r="I29" s="28">
+        <v>412</v>
+      </c>
+      <c r="J29" s="28">
+        <v>367</v>
+      </c>
+      <c r="K29" s="30">
+        <v>1491</v>
+      </c>
+      <c r="L29" s="29">
+        <v>7129</v>
+      </c>
+      <c r="M29" s="28">
+        <v>140</v>
+      </c>
+      <c r="N29" s="28">
+        <v>65</v>
+      </c>
+      <c r="O29" s="35" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" ht="19.2" x14ac:dyDescent="0.25">
+      <c r="B30" s="27" t="s">
+        <v>33</v>
+      </c>
+      <c r="C30" s="28">
+        <v>261</v>
+      </c>
+      <c r="D30" s="28">
+        <v>249</v>
+      </c>
+      <c r="E30" s="28">
+        <v>185</v>
+      </c>
+      <c r="F30" s="28">
+        <v>183</v>
+      </c>
+      <c r="G30" s="30">
+        <v>1990</v>
+      </c>
+      <c r="H30" s="40">
+        <v>2417</v>
+      </c>
+      <c r="I30" s="28">
+        <v>376</v>
+      </c>
+      <c r="J30" s="28">
+        <v>341</v>
+      </c>
+      <c r="K30" s="30">
+        <v>1473</v>
+      </c>
+      <c r="L30" s="29">
+        <v>7293</v>
+      </c>
+      <c r="M30" s="28">
+        <v>124</v>
+      </c>
+      <c r="N30" s="28">
+        <v>63</v>
+      </c>
+      <c r="O30" s="35" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" ht="19.2" x14ac:dyDescent="0.25">
+      <c r="B31" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="C31" s="28">
+        <v>162</v>
+      </c>
+      <c r="D31" s="28">
+        <v>160</v>
+      </c>
+      <c r="E31" s="28">
+        <v>136</v>
+      </c>
+      <c r="F31" s="28">
+        <v>150</v>
+      </c>
+      <c r="G31" s="30">
+        <v>1551</v>
+      </c>
+      <c r="H31" s="28">
+        <v>1121</v>
+      </c>
+      <c r="I31" s="28">
+        <v>334</v>
+      </c>
+      <c r="J31" s="28">
+        <v>296</v>
+      </c>
+      <c r="K31" s="28">
+        <v>809</v>
+      </c>
+      <c r="L31" s="39">
+        <v>3775</v>
+      </c>
+      <c r="M31" s="28">
+        <v>127</v>
+      </c>
+      <c r="N31" s="28">
+        <v>99</v>
+      </c>
+      <c r="O31" s="35" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" ht="19.2" x14ac:dyDescent="0.25">
+      <c r="B32" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="C32" s="28">
+        <v>114</v>
+      </c>
+      <c r="D32" s="28">
+        <v>110</v>
+      </c>
+      <c r="E32" s="28">
+        <v>105</v>
+      </c>
+      <c r="F32" s="28">
+        <v>108</v>
+      </c>
+      <c r="G32" s="28">
+        <v>151</v>
+      </c>
+      <c r="H32" s="30">
+        <v>1255</v>
+      </c>
+      <c r="I32" s="28">
+        <v>240</v>
+      </c>
+      <c r="J32" s="28">
+        <v>271</v>
+      </c>
+      <c r="K32" s="28">
+        <v>760</v>
+      </c>
+      <c r="L32" s="39">
+        <v>3655</v>
+      </c>
+      <c r="M32" s="28">
+        <v>125</v>
+      </c>
+      <c r="N32" s="28">
+        <v>70</v>
+      </c>
+      <c r="O32" s="35" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="33" spans="2:15" ht="19.2" x14ac:dyDescent="0.25">
+      <c r="B33" s="27" t="s">
+        <v>36</v>
+      </c>
+      <c r="C33" s="28">
+        <v>85</v>
+      </c>
+      <c r="D33" s="28">
+        <v>87</v>
+      </c>
+      <c r="E33" s="28">
+        <v>130</v>
+      </c>
+      <c r="F33" s="28">
+        <v>106</v>
+      </c>
+      <c r="G33" s="28">
+        <v>745</v>
+      </c>
+      <c r="H33" s="28">
+        <v>820</v>
+      </c>
+      <c r="I33" s="28">
+        <v>223</v>
+      </c>
+      <c r="J33" s="28">
+        <v>214</v>
+      </c>
+      <c r="K33" s="28">
+        <v>328</v>
+      </c>
+      <c r="L33" s="28">
+        <v>1084</v>
+      </c>
+      <c r="M33" s="28">
+        <v>126</v>
+      </c>
+      <c r="N33" s="28">
+        <v>67</v>
+      </c>
+      <c r="O33" s="35" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="34" spans="2:15" ht="19.2" x14ac:dyDescent="0.25">
+      <c r="B34" s="27" t="s">
+        <v>37</v>
+      </c>
+      <c r="C34" s="28">
+        <v>79</v>
+      </c>
+      <c r="D34" s="28">
+        <v>77</v>
+      </c>
+      <c r="E34" s="28">
+        <v>86</v>
+      </c>
+      <c r="F34" s="28">
+        <v>88</v>
+      </c>
+      <c r="G34" s="28">
+        <v>126</v>
+      </c>
+      <c r="H34" s="28">
+        <v>585</v>
+      </c>
+      <c r="I34" s="28">
+        <v>140</v>
+      </c>
+      <c r="J34" s="28">
+        <v>185</v>
+      </c>
+      <c r="K34" s="28">
+        <v>195</v>
+      </c>
+      <c r="L34" s="28">
+        <v>1069</v>
+      </c>
+      <c r="M34" s="28">
+        <v>129</v>
+      </c>
+      <c r="N34" s="28">
+        <v>67</v>
+      </c>
+      <c r="O34" s="35" t="s">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter alignWithMargins="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A2:O34"/>
   <sheetViews>
@@ -3472,556 +4022,6 @@
       </c>
       <c r="N34" s="28">
         <v>106</v>
-      </c>
-      <c r="O34" s="35" t="s">
-        <v>30</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter alignWithMargins="0"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A2:O34"/>
-  <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G34" sqref="G34"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="20.6640625" style="21" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" style="21" customWidth="1"/>
-    <col min="3" max="16384" width="9.109375" style="21"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="21" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="21" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="21" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="21" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="21" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="21" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="22">
-        <v>44019</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="21" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="23">
-        <v>0.55675925925925929</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="21" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="21" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="21" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="21" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" s="21" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="24" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" s="25"/>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" s="21" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14" s="21" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="21" t="s">
-        <v>19</v>
-      </c>
-      <c r="B15" s="21" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B16" s="21" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B17" s="21" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B18" s="21" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B19" s="21" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B20" s="21" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B21" s="21" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A23" s="24" t="s">
-        <v>27</v>
-      </c>
-      <c r="B23" s="25"/>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A24" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="B24" s="21">
-        <v>23.5</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B26" s="26"/>
-      <c r="C26" s="27">
-        <v>1</v>
-      </c>
-      <c r="D26" s="27">
-        <v>2</v>
-      </c>
-      <c r="E26" s="27">
-        <v>3</v>
-      </c>
-      <c r="F26" s="27">
-        <v>4</v>
-      </c>
-      <c r="G26" s="27">
-        <v>5</v>
-      </c>
-      <c r="H26" s="27">
-        <v>6</v>
-      </c>
-      <c r="I26" s="27">
-        <v>7</v>
-      </c>
-      <c r="J26" s="27">
-        <v>8</v>
-      </c>
-      <c r="K26" s="27">
-        <v>9</v>
-      </c>
-      <c r="L26" s="27">
-        <v>10</v>
-      </c>
-      <c r="M26" s="27">
-        <v>11</v>
-      </c>
-      <c r="N26" s="27">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15" ht="19.2" x14ac:dyDescent="0.25">
-      <c r="B27" s="27" t="s">
-        <v>29</v>
-      </c>
-      <c r="C27" s="28">
-        <v>720</v>
-      </c>
-      <c r="D27" s="28">
-        <v>786</v>
-      </c>
-      <c r="E27" s="28">
-        <v>442</v>
-      </c>
-      <c r="F27" s="28">
-        <v>458</v>
-      </c>
-      <c r="G27" s="30">
-        <v>1970</v>
-      </c>
-      <c r="H27" s="40">
-        <v>2525</v>
-      </c>
-      <c r="I27" s="28">
-        <v>457</v>
-      </c>
-      <c r="J27" s="28">
-        <v>562</v>
-      </c>
-      <c r="K27" s="40">
-        <v>2892</v>
-      </c>
-      <c r="L27" s="33">
-        <v>15462</v>
-      </c>
-      <c r="M27" s="28">
-        <v>125</v>
-      </c>
-      <c r="N27" s="28">
-        <v>61</v>
-      </c>
-      <c r="O27" s="35" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15" ht="19.2" x14ac:dyDescent="0.25">
-      <c r="B28" s="27" t="s">
-        <v>31</v>
-      </c>
-      <c r="C28" s="28">
-        <v>586</v>
-      </c>
-      <c r="D28" s="28">
-        <v>565</v>
-      </c>
-      <c r="E28" s="28">
-        <v>385</v>
-      </c>
-      <c r="F28" s="28">
-        <v>375</v>
-      </c>
-      <c r="G28" s="40">
-        <v>3218</v>
-      </c>
-      <c r="H28" s="39">
-        <v>4203</v>
-      </c>
-      <c r="I28" s="28">
-        <v>528</v>
-      </c>
-      <c r="J28" s="28">
-        <v>477</v>
-      </c>
-      <c r="K28" s="40">
-        <v>2484</v>
-      </c>
-      <c r="L28" s="33">
-        <v>14460</v>
-      </c>
-      <c r="M28" s="28">
-        <v>127</v>
-      </c>
-      <c r="N28" s="28">
-        <v>63</v>
-      </c>
-      <c r="O28" s="35" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="29" spans="1:15" ht="19.2" x14ac:dyDescent="0.25">
-      <c r="B29" s="27" t="s">
-        <v>32</v>
-      </c>
-      <c r="C29" s="28">
-        <v>419</v>
-      </c>
-      <c r="D29" s="28">
-        <v>444</v>
-      </c>
-      <c r="E29" s="28">
-        <v>301</v>
-      </c>
-      <c r="F29" s="28">
-        <v>304</v>
-      </c>
-      <c r="G29" s="30">
-        <v>2210</v>
-      </c>
-      <c r="H29" s="40">
-        <v>2780</v>
-      </c>
-      <c r="I29" s="28">
-        <v>412</v>
-      </c>
-      <c r="J29" s="28">
-        <v>367</v>
-      </c>
-      <c r="K29" s="30">
-        <v>1491</v>
-      </c>
-      <c r="L29" s="29">
-        <v>7129</v>
-      </c>
-      <c r="M29" s="28">
-        <v>140</v>
-      </c>
-      <c r="N29" s="28">
-        <v>65</v>
-      </c>
-      <c r="O29" s="35" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="30" spans="1:15" ht="19.2" x14ac:dyDescent="0.25">
-      <c r="B30" s="27" t="s">
-        <v>33</v>
-      </c>
-      <c r="C30" s="28">
-        <v>261</v>
-      </c>
-      <c r="D30" s="28">
-        <v>249</v>
-      </c>
-      <c r="E30" s="28">
-        <v>185</v>
-      </c>
-      <c r="F30" s="28">
-        <v>183</v>
-      </c>
-      <c r="G30" s="30">
-        <v>1990</v>
-      </c>
-      <c r="H30" s="40">
-        <v>2417</v>
-      </c>
-      <c r="I30" s="28">
-        <v>376</v>
-      </c>
-      <c r="J30" s="28">
-        <v>341</v>
-      </c>
-      <c r="K30" s="30">
-        <v>1473</v>
-      </c>
-      <c r="L30" s="29">
-        <v>7293</v>
-      </c>
-      <c r="M30" s="28">
-        <v>124</v>
-      </c>
-      <c r="N30" s="28">
-        <v>63</v>
-      </c>
-      <c r="O30" s="35" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15" ht="19.2" x14ac:dyDescent="0.25">
-      <c r="B31" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="C31" s="28">
-        <v>162</v>
-      </c>
-      <c r="D31" s="28">
-        <v>160</v>
-      </c>
-      <c r="E31" s="28">
-        <v>136</v>
-      </c>
-      <c r="F31" s="28">
-        <v>150</v>
-      </c>
-      <c r="G31" s="30">
-        <v>1551</v>
-      </c>
-      <c r="H31" s="28">
-        <v>1121</v>
-      </c>
-      <c r="I31" s="28">
-        <v>334</v>
-      </c>
-      <c r="J31" s="28">
-        <v>296</v>
-      </c>
-      <c r="K31" s="28">
-        <v>809</v>
-      </c>
-      <c r="L31" s="39">
-        <v>3775</v>
-      </c>
-      <c r="M31" s="28">
-        <v>127</v>
-      </c>
-      <c r="N31" s="28">
-        <v>99</v>
-      </c>
-      <c r="O31" s="35" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="32" spans="1:15" ht="19.2" x14ac:dyDescent="0.25">
-      <c r="B32" s="27" t="s">
-        <v>35</v>
-      </c>
-      <c r="C32" s="28">
-        <v>114</v>
-      </c>
-      <c r="D32" s="28">
-        <v>110</v>
-      </c>
-      <c r="E32" s="28">
-        <v>105</v>
-      </c>
-      <c r="F32" s="28">
-        <v>108</v>
-      </c>
-      <c r="G32" s="28">
-        <v>151</v>
-      </c>
-      <c r="H32" s="30">
-        <v>1255</v>
-      </c>
-      <c r="I32" s="28">
-        <v>240</v>
-      </c>
-      <c r="J32" s="28">
-        <v>271</v>
-      </c>
-      <c r="K32" s="28">
-        <v>760</v>
-      </c>
-      <c r="L32" s="39">
-        <v>3655</v>
-      </c>
-      <c r="M32" s="28">
-        <v>125</v>
-      </c>
-      <c r="N32" s="28">
-        <v>70</v>
-      </c>
-      <c r="O32" s="35" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="33" spans="2:15" ht="19.2" x14ac:dyDescent="0.25">
-      <c r="B33" s="27" t="s">
-        <v>36</v>
-      </c>
-      <c r="C33" s="28">
-        <v>85</v>
-      </c>
-      <c r="D33" s="28">
-        <v>87</v>
-      </c>
-      <c r="E33" s="28">
-        <v>130</v>
-      </c>
-      <c r="F33" s="28">
-        <v>106</v>
-      </c>
-      <c r="G33" s="28">
-        <v>745</v>
-      </c>
-      <c r="H33" s="28">
-        <v>820</v>
-      </c>
-      <c r="I33" s="28">
-        <v>223</v>
-      </c>
-      <c r="J33" s="28">
-        <v>214</v>
-      </c>
-      <c r="K33" s="28">
-        <v>328</v>
-      </c>
-      <c r="L33" s="28">
-        <v>1084</v>
-      </c>
-      <c r="M33" s="28">
-        <v>126</v>
-      </c>
-      <c r="N33" s="28">
-        <v>67</v>
-      </c>
-      <c r="O33" s="35" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="34" spans="2:15" ht="19.2" x14ac:dyDescent="0.25">
-      <c r="B34" s="27" t="s">
-        <v>37</v>
-      </c>
-      <c r="C34" s="28">
-        <v>79</v>
-      </c>
-      <c r="D34" s="28">
-        <v>77</v>
-      </c>
-      <c r="E34" s="28">
-        <v>86</v>
-      </c>
-      <c r="F34" s="28">
-        <v>88</v>
-      </c>
-      <c r="G34" s="28">
-        <v>126</v>
-      </c>
-      <c r="H34" s="28">
-        <v>585</v>
-      </c>
-      <c r="I34" s="28">
-        <v>140</v>
-      </c>
-      <c r="J34" s="28">
-        <v>185</v>
-      </c>
-      <c r="K34" s="28">
-        <v>195</v>
-      </c>
-      <c r="L34" s="28">
-        <v>1069</v>
-      </c>
-      <c r="M34" s="28">
-        <v>129</v>
-      </c>
-      <c r="N34" s="28">
-        <v>67</v>
       </c>
       <c r="O34" s="35" t="s">
         <v>30</v>

</xml_diff>